<commit_message>
made required changes in  excel files
</commit_message>
<xml_diff>
--- a/Bavdhan-cleaned.xlsx
+++ b/Bavdhan-cleaned.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4299" uniqueCount="1930">
   <si>
-    <t xml:space="preserve">Title</t>
+    <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">off</t>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">ratings</t>
   </si>
   <si>
-    <t xml:space="preserve">price_for_1</t>
+    <t xml:space="preserve">price_for_one</t>
   </si>
   <si>
     <t xml:space="preserve">delivery_reviews</t>
@@ -5980,7 +5980,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -6002,12 +6002,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -6057,7 +6051,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6084,13 +6078,13 @@
   </sheetPr>
   <dimension ref="A1:F835"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A812" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E843" activeCellId="0" sqref="E843"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.64"/>

</xml_diff>